<commit_message>
Updated BVT of 22 visuals
</commit_message>
<xml_diff>
--- a/documents/Published/Box and Whisker/BoxAndWhiskerByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Box and Whisker/BoxAndWhiskerByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI-CustomVisuals\documents\Published\BoxAndWhisker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLab_PowerBIVisuals\documents\Published\BoxAndWhisker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DD3440-92B3-450F-A4CB-3BE44BA08B82}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51111B3-3F9B-4FBA-B538-47150D74C83D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="308">
   <si>
     <t>S no</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Add legend to the visual</t>
-  </si>
-  <si>
-    <t>Add gradient to the visual</t>
   </si>
   <si>
     <t>Tooltips</t>
@@ -463,12 +460,6 @@
     <t>Check whether Legend title ON/OFF button is working or not</t>
   </si>
   <si>
-    <t>1. Go to formatting pane
-2. Go to Legend
-3. Update Title button to 'OFF'
-4. Update Title button to 'ON'</t>
-  </si>
-  <si>
     <t>1. Legend title should not be displayed in the visual when the button is in 'OFF' state
 2. Legend title should be displayed in the visual when the button is in 'ON' state</t>
   </si>
@@ -513,10 +504,6 @@
   </si>
   <si>
     <t>Highlight</t>
-  </si>
-  <si>
-    <t>1. Drag 'GPA' column in 'Legend' field
-2. Apply sum aggregation to the 'GPA' column</t>
   </si>
   <si>
     <t>Labels should not be split from the axis</t>
@@ -677,9 +664,6 @@
     <t>Update color of Y-Axis labels</t>
   </si>
   <si>
-    <t>Color of dots is based on the gradient</t>
-  </si>
-  <si>
     <t>Legend will be added to the visual and color of dots is based on the legend</t>
   </si>
   <si>
@@ -1228,6 +1212,11 @@
 2. Visual will update according to selections
 3. In the boomarks pane, a new entry of the bookmark will come
 4. The selection state saved in bookmark will be restored in the visual</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Switch Legend toggle to 'OFF'
+4. Switch Legend toggle to 'ON'</t>
   </si>
 </sst>
 </file>
@@ -1396,6 +1385,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1413,15 +1411,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1737,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD979CE-A2F4-4A57-BF74-C680FEBF31B0}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,7 +1756,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1778,13 +1767,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1795,26 +1784,26 @@
         <v>5</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="14"/>
       <c r="C4" s="13" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1825,13 +1814,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1839,19 +1828,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1859,320 +1848,324 @@
         <v>10</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>11</v>
+        <v>276</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>161</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>288</v>
+        <v>16</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>7</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>158</v>
+      </c>
       <c r="C11" s="13" t="s">
-        <v>16</v>
+        <v>159</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>158</v>
+        <v>160</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>8</v>
-      </c>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="D12" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="E12" s="15" t="s">
         <v>164</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="E14" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="15" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>9</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
         <v>172</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="13" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>9</v>
-      </c>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="D16" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="E17" s="13" t="s">
         <v>180</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="E18" s="13" t="s">
         <v>183</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="13" t="s">
         <v>186</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="E20" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="E21" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>195</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>198</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="E24" s="13" t="s">
         <v>201</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="E25" s="13" t="s">
         <v>204</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="E27" s="13" t="s">
         <v>210</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>213</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="E29" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E29" s="13" t="s">
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>10</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
         <v>218</v>
       </c>
@@ -2184,99 +2177,95 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
-        <v>10</v>
-      </c>
-      <c r="B31" s="13" t="s">
+      <c r="A31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="E31" s="13" t="s">
         <v>223</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="E32" s="13" t="s">
         <v>226</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="E33" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="13"/>
+    </row>
+    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>11</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="C34" s="13" t="s">
-        <v>231</v>
+        <v>19</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>232</v>
+        <v>20</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>233</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
-        <v>11</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>19</v>
-      </c>
+      <c r="A35" s="11"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="14"/>
       <c r="C36" s="13" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="14"/>
       <c r="C37" s="13" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>29</v>
@@ -2286,260 +2275,264 @@
       <c r="A38" s="11"/>
       <c r="B38" s="14"/>
       <c r="C38" s="13" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="14"/>
       <c r="C39" s="13" t="s">
-        <v>32</v>
+        <v>230</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>33</v>
+        <v>231</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>52</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="14"/>
       <c r="C40" s="13" t="s">
-        <v>234</v>
+        <v>34</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>235</v>
+        <v>39</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="14"/>
       <c r="C41" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D41" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="14"/>
       <c r="C42" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>41</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="14"/>
       <c r="C43" s="13" t="s">
-        <v>39</v>
+        <v>233</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>42</v>
+        <v>234</v>
       </c>
       <c r="E43" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>12</v>
+      </c>
+      <c r="B44" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="14"/>
       <c r="C44" s="13" t="s">
-        <v>237</v>
+        <v>69</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>238</v>
+        <v>44</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
-        <v>12</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>44</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="13" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="14"/>
       <c r="C46" s="13" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="14"/>
       <c r="C47" s="13" t="s">
-        <v>49</v>
+        <v>236</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>50</v>
+        <v>237</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>51</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="14"/>
       <c r="C48" s="13" t="s">
-        <v>240</v>
+        <v>52</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>241</v>
+        <v>58</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>242</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="14"/>
       <c r="C49" s="13" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="14"/>
       <c r="C50" s="13" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="14"/>
       <c r="C51" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>57</v>
+        <v>239</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="14"/>
       <c r="C52" s="13" t="s">
-        <v>56</v>
+        <v>241</v>
       </c>
       <c r="D52" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E52" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="E52" s="13" t="s">
+    </row>
+    <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>13</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="13" t="s">
+      <c r="D54" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="E54" s="13" t="s">
         <v>246</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="11">
-        <v>13</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
-      <c r="B55" s="13"/>
+      <c r="B55" s="14"/>
       <c r="C55" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>14</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D56" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E56" s="13" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>251</v>
@@ -2555,425 +2548,408 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="11">
-        <v>15</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>255</v>
-      </c>
+      <c r="A58" s="11"/>
+      <c r="B58" s="14"/>
       <c r="C58" s="13" t="s">
-        <v>256</v>
+        <v>70</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>257</v>
+        <v>71</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="14"/>
       <c r="C59" s="13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
-      <c r="B60" s="14"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
+        <v>16</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="C60" s="13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A61" s="11">
-        <v>16</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>77</v>
-      </c>
+      <c r="A61" s="11"/>
+      <c r="B61" s="14"/>
       <c r="C61" s="13" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D61" s="13" t="s">
         <v>83</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="14"/>
       <c r="C62" s="13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="14"/>
       <c r="C63" s="13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="14"/>
+      <c r="A64" s="11">
+        <v>17</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>88</v>
+      </c>
       <c r="C64" s="13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E64" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E65" s="13" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="11">
-        <v>17</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E65" s="13" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="14"/>
       <c r="C66" s="13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="14"/>
       <c r="C67" s="13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
-      <c r="B68" s="14"/>
+      <c r="A68" s="11">
+        <v>18</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>255</v>
+      </c>
       <c r="C68" s="13" t="s">
-        <v>99</v>
+        <v>256</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>100</v>
+        <v>257</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="11">
-        <v>18</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="A69" s="11"/>
+      <c r="B69" s="13"/>
       <c r="C69" s="13" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D71" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="E71" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="E71" s="13" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
+    </row>
+    <row r="72" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="11"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D73" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="D72" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>269</v>
-      </c>
       <c r="E73" s="13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="14"/>
+      <c r="A74" s="11">
+        <v>19</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="C74" s="13" t="s">
-        <v>291</v>
+        <v>102</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>270</v>
+        <v>103</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="11">
-        <v>19</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>10</v>
-      </c>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" s="11"/>
+      <c r="B75" s="14"/>
       <c r="C75" s="13" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="14"/>
       <c r="C76" s="13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="14"/>
       <c r="C77" s="13" t="s">
-        <v>109</v>
+        <v>267</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>110</v>
+        <v>268</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>111</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="14"/>
       <c r="C78" s="13" t="s">
-        <v>271</v>
+        <v>111</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>272</v>
+        <v>307</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>273</v>
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="14"/>
       <c r="C79" s="13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D79" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E79" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E79" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="14"/>
       <c r="C80" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="14"/>
       <c r="C81" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D81" s="13" t="s">
         <v>119</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="14"/>
       <c r="C82" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="11">
+        <v>20</v>
+      </c>
+      <c r="B83" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D82" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="E82" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
-      <c r="B83" s="14"/>
       <c r="C83" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="11"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="11">
+        <v>21</v>
+      </c>
+      <c r="B85" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D83" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E83" s="13" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="11">
-        <v>20</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="D84" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="E84" s="13" t="s">
+      <c r="C85" s="13" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="13" t="s">
+      <c r="D85" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="E85" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="D85" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="E85" s="13" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="11">
-        <v>21</v>
-      </c>
-      <c r="B86" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="D86" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="E86" s="13" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A87" s="23">
+    </row>
+    <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="17">
         <v>22</v>
       </c>
-      <c r="B87" s="22" t="s">
-        <v>307</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>308</v>
-      </c>
-      <c r="D87" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="E87" s="24" t="s">
-        <v>310</v>
+      <c r="B86" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2997,13 +2973,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3011,10 +2987,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3022,10 +2998,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3033,10 +3009,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3044,10 +3020,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3055,10 +3031,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3066,10 +3042,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3077,10 +3053,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3088,10 +3064,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3099,10 +3075,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3110,10 +3086,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3121,10 +3097,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3132,10 +3108,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3143,10 +3119,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3154,10 +3130,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3165,94 +3141,94 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="23"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C18" s="20"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="23"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="C23" s="23"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="23"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" s="20"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" s="20"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="20"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="24"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>19</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3260,10 +3236,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>